<commit_message>
arreglando error de duplicados
</commit_message>
<xml_diff>
--- a/entrada/acumulador.xlsx
+++ b/entrada/acumulador.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A235"/>
+  <dimension ref="A1:A306"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -982,21 +982,21 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>COL-00-02-00 0 26/01/2024</t>
+          <t>COL-AB-02-00 0 26/01/2024</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>COLUMPIO ARCO Medidas Capacidad Área Mínima Edad (años)</t>
+          <t>COLUMPIO PP EN A CON 3 Medidas Capacidad Área Mínima Edad (años)</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>3.95m x 1.30m x 2.55m 2 niños 9.60m x 4.90m 4-12</t>
+          <t>ASIENTOS DE BANDA 3.30m x 1.60m x 2.7 0m 3 niños 7.00m x 5.20m 4-12</t>
         </is>
       </c>
     </row>
@@ -1010,742 +1010,742 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Columpio fabricado con tubo redondo NGR Ced.30 y</t>
+          <t>Juego formado por 2 tijeras curvas de diámetro, un</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Norma ASTM-A-513, se ubican 2 bandas para parque</t>
+          <t>travesaño en tubo redondo NGR 2” de diámetro Ced.40</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>público sujetadas con 2 cadenas galvanizadas de ¼”,</t>
+          <t>Norma ASTM-A-513 y 3 columpios con cadena galvanizada</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>ganchos. El movimiento del columpio es realizado por</t>
+          <t>1/4” grado 30 formada en frio con eslabones electro-</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>pénduloconcentrodebronceparaevitareldesgaste.</t>
+          <t>soldados,cuentaconpénduloybandoladeaceroinoxidable,</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Sujeción y Unión</t>
+          <t>asítambiéncuentacon accesorios fabricadosenplásticode</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>UtilizacióndesoldaduraMIGG(GMAW),paralauniónde</t>
+          <t>importación americanacomo:Canastillas deBanda.Eneste</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>los elementos de un componente en acero. Sujeción</t>
+          <t>columpio adquieren destreza motriz y cultivan diversas</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>accesoriosmediantetornillostipo"Torks",tuercasinserto</t>
+          <t>habilidades, para que los niños jueguen y se diviertan</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>nylon, tuercas de presión y aplicación de "LocTite”, lo</t>
+          <t>durantehoras,coloraelegir.</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>cualdificultalaextracciónyelvandalismo.</t>
+          <t>Sujeción y Unión</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Recubrimiento</t>
+          <t>UtilizacióndesoldaduraMIGG(GMAW),paralauniónde</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Las partes en acero pasan por un tratamiento de</t>
+          <t>los elementos de un componente en acero. Sujeción</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>superficie de tres etapas para evitar la oxidación natural</t>
+          <t>accesoriosmediantetornillostipo"Torks",tuercasinserto</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>del acero: Fosfatodesengrase, enjuague y sellado, el</t>
+          <t>nylon, tuercas de presión y aplicación de "LocTite”, lo</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>cualevitalaoxidaciónnaturaldelacero.Selesaplicaun</t>
+          <t>cualdificultalaextracciónyelvandalismo.</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>recubrimiento de pintura poliésterelectrostático en polvo</t>
+          <t>Recubrimiento</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>(PowderCoating) con una temperatura de curado a 200°</t>
+          <t>Las partes en acero pasan por un tratamiento de</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>C. lo cualasegurala adherencia,la dureza yel brillo del</t>
+          <t>superficie de tres etapas para evitar la oxidación natural</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>recubrimientosobreelproducto.</t>
+          <t>del acero: Fosfatodesengrase, enjuague y sellado, el</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Imagen de referencia, puede haber variación</t>
+          <t>cualevitalaoxidaciónnaturaldelacero.Selesaplicaun</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>2.55m</t>
+          <t>recubrimiento de pintura poliéster electrostático en polvo</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>3.95m</t>
+          <t>(PowderCoating) con una temperatura de curado a 200°</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>1.30m</t>
+          <t>C. lo cualasegurala adherencia,la dureza yel brillo del</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Dimensiones de referencia, puede haber variaciones.</t>
+          <t>Imagen de referencia, puede haber variación</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>VARIANTES DE ANCLAJE</t>
+          <t>recubrimientosobreelproducto.</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>ANCLADO EN CEMENTO:</t>
+          <t>2.70m</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>TAQUETEADO</t>
+          <t>3.30m</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>• Realizar hoyos de 40cm de</t>
+          <t>1.60m</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>• Elconcretoausardebeserde200Kg/cm2 Diámetro.</t>
+          <t>Dimensiones de referencia, puede haber variaciones.</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>deresistencia. • Excavara30cmdeprofundidadpara</t>
+          <t>VARIANTES DE ANCLAJE</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>• El espesor mínimo de la plancha de enterrarpostesyaccesorios.</t>
+          <t>ANCLADO EN CEMENTO:</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>concretodebeserde15cm. • Rellenar hoyos con un concreto de</t>
+          <t>TAQUETEADO</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>• Usartaquetesexpansivosde3/8”x3¾”. 200Kg/cm2deresistencia.</t>
+          <t>• Realizar hoyos de 40cm de</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>COL-AB-01-00 0 26/01/2024</t>
+          <t>• Elconcretoausardebeserde200Kg/cm2 Diámetro.</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>COLUMPIO PP EN A CON 2 Medidas Capacidad Área Mínima Edad (años)</t>
+          <t>deresistencia. • Excavara30cmdeprofundidadpara</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>ASIENTOS DE BANDA 2.70m x 1.60m x 2.70m 2 niños 5.90m x 5.20m 1.5-3</t>
+          <t>• El espesor mínimo de la plancha de enterrarpostesyaccesorios.</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Descripción de producto</t>
+          <t>concretodebeserde15cm. • Rellenar hoyos con un concreto de</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Columpios para 2 personas con asientos de bandas plástica</t>
+          <t>• Usartaquetesexpansivosde3/8”x3¾”. 200Kg/cm2deresistencia.</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>de uso rudo, colgadas con cadenas galvanizadas sobre un</t>
+          <t>COL-AB-03-00 0 27/12/2023</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>travesaño y tijeras curvas de tubo redondo NGR Ced.30</t>
+          <t>COLUMPIO PP EN U CON Medidas Capacidad Área segura Edad (años)</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Norma ASTM-A-513</t>
+          <t>3 ASIENTOS DE BANDA 3.20m x 1.30m x 2.60m 3niños 6.70m x 4.80m 4-12 años</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>El movimiento del columpio es realizado por péndulo con</t>
+          <t>Descripción de producto</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>centro de bronce para evitar el desgaste.</t>
+          <t>Columpio con diseño en forma de arcos está</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Sujeción y Unión</t>
+          <t>fabricado con tubo redondo NGR Ced.30 y</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Utilización de soldadura MIGG (GMAW), para la unión de</t>
+          <t>Norma ASTM-A-513, su travesaño de tubo</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>los elementos de un componente en acero. Sujeción</t>
+          <t>redondo NGR Ced.40 Norma ASTM-A-513, en la</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>accesorios mediante tornillos tipo "Torks", tuercas inserto</t>
+          <t>cual se ubican 3 bandas para parque público</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>nylon, tuercas de presión y aplicación de "LocTite”, lo cual</t>
+          <t>sujetadas con 6 cadenas galvanizadas de 1/4”,</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>dificulta la extracción y el vandalismo.</t>
+          <t>ganchos y péndulos el cual le permite el</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Recubrimiento</t>
+          <t>movimiento.</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Las partes en acero pasan por un tratamiento de superficie</t>
+          <t>Sujeción y Unión</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>de tres etapas para evitar la oxidación natural del acero:</t>
+          <t>Utilización de soldadura MIGG (GMAW), para la</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Fosfatodesengrase, enjuague y sellado, el cual evita la</t>
+          <t>unión de los elementos de un componente en</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>oxidación natural del acero. Se les aplica un recubrimiento</t>
+          <t>acero. Sujeción accesorios mediante tornillos tipo</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>de pintura poliéster electrostático en polvo (PowderCoating)</t>
+          <t>"Torks",tuercasinsertonylon,tuercasdepresióny</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>con una temperatura de curado a 200° C. lo cual asegura la</t>
+          <t>aplicación de "LocTite”, lo cual dificulta la</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>adherencia, la dureza y el brillo del recubrimiento sobre el</t>
+          <t>extracciónyelvandalismo.</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>producto.</t>
+          <t>Imagen de referencia, puede haber variación</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Imagen de referencia, puede haber variación</t>
+          <t>Recubrimiento</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>2.70m</t>
+          <t>Laspartesenaceropasanporuntratamientode</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>2.70m</t>
+          <t>superficie de tres etapasparaevitar la oxidación</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>1.60m</t>
+          <t>natural del acero: Fosfatodesengrase, enjuague</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Dimensiones de referencia, puede haber variaciones.</t>
+          <t>y sellado, el cual evita la oxidación natural del</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>VARIANTES DE ANCLAJE</t>
+          <t>2.60m 1.30m</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>ANCLADO EN CEMENTO:</t>
+          <t>acero. Se les aplica un recubrimiento de pintura</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>TAQUETEADO</t>
+          <t>poliésterelectrostáticoenpolvo(PowderCoating)</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>• Realizar hoyos de 40cm de</t>
+          <t>3.20m conunatemperaturadecuradoa200°C.locual</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>• El concreto a usar debe ser de 200 Kg/cm2 Diámetro.</t>
+          <t>asegura la adherencia, la dureza y el brillo del</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>de resistencia. • Excavar a 30cm de profundidad para</t>
+          <t>recubrimientosobreelproducto.</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>• El espesor mínimo de la plancha de enterrar postes y accesorios.</t>
+          <t>Dimensiones de referencia, puede haber variaciones.</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>concreto debe ser de 15cm. • Rellenar hoyos con un concreto de</t>
+          <t>• Realizarhoyosde40cmdeDiámetro.</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>• Usar taquetes expansivos de 3/8” x 3 ¾ ”. 200Kg/cm2 de resistencia.</t>
+          <t>ANCLADO EN CEMENTO: • Excavar a 30cm de profundidad para enterrar</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>COL-AB-02-00 0 26/01/2024</t>
+          <t>postesyaccesorios.</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>COLUMPIO PP EN A CON 3 Medidas Capacidad Área Mínima Edad (años)</t>
+          <t>• Rellenarhoyosconunconcretode200Kg/cm2</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>ASIENTOS DE BANDA 3.30m x 1.60m x 2.7 0m 3 niños 7.00m x 5.20m 4-12</t>
+          <t>deresistencia.</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Descripción de producto</t>
+          <t>COL-AB-04-00 0 09/01/2024</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Juego formado por 2 tijeras curvas de diámetro, un</t>
+          <t>COLUMPIO PP EN A CON Medidas Capacidad Área segura Edad (años)</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>travesaño en tubo redondo NGR 2” de diámetro Ced.40</t>
+          <t>4 ASIENTOS DE BANDA 4.30m x 1.60m x 2.70m 4 niños 6.40m x 3.20m 4-12 años</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Norma ASTM-A-513 y 3 columpios con cadena galvanizada</t>
+          <t>Descripción de producto</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>1/4” grado 30 formada en frio con eslabones electro-</t>
+          <t>Columpio 4 canastillas. en plástico y cadena</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>soldados,cuentaconpénduloybandoladeaceroinoxidable,</t>
+          <t>galvanizada de ¼” . Esta fabricado en tubo</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>asítambiéncuentacon accesorios fabricadosenplásticode</t>
+          <t>redondo NGR Ced.30 Norma ASTM-A-513. El</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>importación americanacomo:Canastillas deBanda.Eneste</t>
+          <t>movimiento del columpio es realizado por</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>columpio adquieren destreza motriz y cultivan diversas</t>
+          <t>péndulo con centro de bronce para evitar el</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>habilidades, para que los niños jueguen y se diviertan</t>
+          <t>desgaste.</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>durantehoras,coloraelegir.</t>
+          <t>Sujeción y Unión</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Sujeción y Unión</t>
+          <t>Utilización de soldadura MIGG (GMAW), para la</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>UtilizacióndesoldaduraMIGG(GMAW),paralauniónde</t>
+          <t>unión de los elementos de un componente en</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>los elementos de un componente en acero. Sujeción</t>
+          <t>acero. Sujeción accesorios mediante tornillos tipo</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>accesoriosmediantetornillostipo"Torks",tuercasinserto</t>
+          <t>"Torks",tuercasinsertonylon,tuercasdepresióny</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>nylon, tuercas de presión y aplicación de "LocTite”, lo</t>
+          <t>aplicación de "LocTite”, lo cual dificulta la</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>cualdificultalaextracciónyelvandalismo.</t>
+          <t>extracciónyelvandalismo.</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>Recubrimiento</t>
+          <t>Imagen de referencia, puede haber variación</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Las partes en acero pasan por un tratamiento de</t>
+          <t>Recubrimiento</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>superficie de tres etapas para evitar la oxidación natural</t>
+          <t>Las partes en acero pasan por un tratamiento de</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>del acero: Fosfatodesengrase, enjuague y sellado, el</t>
+          <t>superficie de tres etapas para evitar la oxidación</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>cualevitalaoxidaciónnaturaldelacero.Selesaplicaun</t>
+          <t>natural del acero: Fosfatodesengrase, enjuague y</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>recubrimiento de pintura poliéster electrostático en polvo</t>
+          <t>2.70m</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>(PowderCoating) con una temperatura de curado a 200°</t>
+          <t>sellado,elcualevitalaoxidaciónnaturaldelacero.</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>C. lo cualasegurala adherencia,la dureza yel brillo del</t>
+          <t>Se les aplica un recubrimiento de pintura poliéster</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>Imagen de referencia, puede haber variación</t>
+          <t>electrostático en polvo (PowderCoating) con una</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>recubrimientosobreelproducto.</t>
+          <t>temperaturadecuradoa200°C.locualasegurala</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>2.70m</t>
+          <t>1.60m 4.30m</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>3.30m</t>
+          <t>adherencia, la dureza y el brillo del recubrimiento</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>1.60m</t>
+          <t>sobreelproducto.</t>
         </is>
       </c>
     </row>
@@ -1759,322 +1759,819 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>VARIANTES DE ANCLAJE</t>
+          <t>• Realizar hoyos de 40cm de Diámetro.</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>ANCLADO EN CEMENTO:</t>
+          <t>• Excavar a 30cm de profundidad para enterrar</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>TAQUETEADO</t>
+          <t>ANCLADO EN CEMENTO:</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>• Realizar hoyos de 40cm de</t>
+          <t>postes y accesorios.</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>• Elconcretoausardebeserde200Kg/cm2 Diámetro.</t>
+          <t>• Rellenar hoyos con un concreto de 200Kg/cm2 de</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>deresistencia. • Excavara30cmdeprofundidadpara</t>
+          <t>resistencia.</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>• El espesor mínimo de la plancha de enterrarpostesyaccesorios.</t>
+          <t>COL-AB-04-01 0 22/07/2024</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>concretodebeserde15cm. • Rellenar hoyos con un concreto de</t>
+          <t>COLUMPIO EN A CON 4 Medidas Capacidad Área Mínima Edad (años)</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>• Usartaquetesexpansivosde3/8”x3¾”. 200Kg/cm2deresistencia.</t>
+          <t>ASIENTOS DE BANDA Y 4.35m x 1.40m x 2.10m 4 niños 7.30m x 5.90m 5-12</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>COL-AB-03-00 0 27/12/2023</t>
+          <t>LATERAL PLASTIPANEL</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>COLUMPIO PP EN U CON Medidas Capacidad Área segura Edad (años)</t>
+          <t>Descripción de producto</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>3 ASIENTOS DE BANDA 3.20m x 1.30m x 2.60m 3niños 6.70m x 4.80m 4-12 años</t>
+          <t>Columpio 4 asientos banda en plástico y cadena galvanizada</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>Descripción de producto</t>
+          <t>de ¼”. Esta fabricado en tubo redondo NGR Ced.30 Norma</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>Columpio con diseño en forma de arcos está</t>
+          <t>ASTM-A-513. El movimiento del columpio es realizado por</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>fabricado con tubo redondo NGR Ced.30 y</t>
+          <t>péndulo con centro de bronce para evitar el desgaste.</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>Norma ASTM-A-513, su travesaño de tubo</t>
+          <t>Sujeción y Unión</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>redondo NGR Ced.40 Norma ASTM-A-513, en la</t>
+          <t>Utilización de soldadura MIGG (GMAW), para la unión de</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>cual se ubican 3 bandas para parque público</t>
+          <t>los elementos de un componente en acero. Sujeción</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>sujetadas con 6 cadenas galvanizadas de 1/4”,</t>
+          <t>accesorios mediante tornillos tipo "Torks", tuercas inserto</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>ganchos y péndulos el cual le permite el</t>
+          <t>nylon, tuercas de presión y aplicación de "LocTite”, lo cual</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>movimiento.</t>
+          <t>dificulta la extracción y el vandalismo.</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>Sujeción y Unión</t>
+          <t>Recubrimiento</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>Utilización de soldadura MIGG (GMAW), para la</t>
+          <t>Las partes en acero pasan por un tratamiento de superficie</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>unión de los elementos de un componente en</t>
+          <t>de tres etapas para evitar la oxidación natural del acero:</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>acero. Sujeción accesorios mediante tornillos tipo</t>
+          <t>Fosfatodesengrase, enjuague y sellado, el cual evita la</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>"Torks",tuercasinsertonylon,tuercasdepresióny</t>
+          <t>oxidación natural del acero. Se les aplica un recubrimiento</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>aplicación de "LocTite”, lo cual dificulta la</t>
+          <t>de pintura poliéster electrostático en polvo (PowderCoating)</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>extracciónyelvandalismo.</t>
+          <t>con una temperatura de curado a 200° C. lo cual asegura la</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>Imagen de referencia, puede haber variación</t>
+          <t>adherencia, la dureza y el brillo del recubrimiento sobre el</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>Recubrimiento</t>
+          <t>producto.</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>Laspartesenaceropasanporuntratamientode</t>
+          <t>Imagen de referencia, puede haber variación</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>superficie de tres etapasparaevitar la oxidación</t>
+          <t>2.10m</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>natural del acero: Fosfatodesengrase, enjuague</t>
+          <t>1.40m 4.35m</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>y sellado, el cual evita la oxidación natural del</t>
+          <t>Dimensiones de referencia, puede haber variaciones.</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>2.60m 1.30m</t>
+          <t>VARIANTES DE ANCLAJE</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>acero. Se les aplica un recubrimiento de pintura</t>
+          <t>ANCLADO EN CEMENTO:</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>poliésterelectrostáticoenpolvo(PowderCoating)</t>
+          <t>TAQUETEADO</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>3.20m conunatemperaturadecuradoa200°C.locual</t>
+          <t>• Realizar hoyos de 40cm de</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>asegura la adherencia, la dureza y el brillo del</t>
+          <t>• El concreto a usar debe ser de 200 Kg/cm2 Diámetro.</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>recubrimientosobreelproducto.</t>
+          <t>de resistencia. • Excavar a 30cm de profundidad para</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>Dimensiones de referencia, puede haber variaciones.</t>
+          <t>• El espesor mínimo de la plancha de enterrar postes y accesorios.</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>• Realizarhoyosde40cmdeDiámetro.</t>
+          <t>concreto debe ser de 15cm. • Rellenar hoyos con un concreto de</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>ANCLADO EN CEMENTO: • Excavar a 30cm de profundidad para enterrar</t>
+          <t>• Usar taquetes expansivos de 3/8” x 3 ¾ ”. 200Kg/cm2 de resistencia.</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>postesyaccesorios.</t>
+          <t>COL-AB-06-00 0 22/07/2024</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>• Rellenarhoyosconunconcretode200Kg/cm2</t>
+          <t>COLUMPIO KRONE Medidas Capacidad Área Mínima Edad (años)</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>deresistencia.</t>
+          <t>6.00m x 5.20m x 2.30m 6niños 9.60m x 8.80m 4-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>Descripción de producto</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>Columpios fabricados en tubo redondo NGR Ced.30 y</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>asientos de bandas, colgándose de cadenas galvanizadas</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>sobre travesaños curvos de tubo redondo NGR Ced.30</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>Norma ASTM-A-513. con cientos de banda de plástico El</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>movimiento del columpio es realizado por péndulo con</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>centro de bronce para evitar el desgaste.</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>Sujeción y Unión</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>Utilización de soldadura MIGG (GMAW), para la unión de</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>los elementos de un componente en acero. Sujeción</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>accesorios mediante tornillos tipo "Torks", tuercas inserto</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>nylon, tuercas de presión y aplicación de "LocTite”, lo cual</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>dificulta la extracción y el vandalismo.</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>Recubrimiento</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>Las partes en acero pasan por un tratamiento de superficie</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>de tres etapas para evitar la oxidación natural del acero:</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>Fosfatodesengrase, enjuague y sellado, el cual evita la</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>oxidación natural del acero. Se les aplica un recubrimiento</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>de pintura poliéster electrostático en polvo (PowderCoating)</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>con una temperatura de curado a 200° C. lo cual asegura la</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>Imagen de referencia, puede haber variación adherencia, la dureza y el brillo del recubrimiento sobre el</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>producto.</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>2.10m</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>1.25m 2.74m</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>Dimensiones de referencia, puede haber variaciones.</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>VARIANTES DE ANCLAJE</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>ANCLADO EN CEMENTO:</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>TAQUETEADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>• Realizar hoyos de 40cm de</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>• El concreto a usar debe ser de 200 Kg/cm2 Diámetro.</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>de resistencia. • Excavar a 30cm de profundidad para</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>• El espesor mínimo de la plancha de enterrar postes y accesorios.</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>concreto debe ser de 15cm. • Rellenar hoyos con un concreto de</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>• Usar taquetes expansivos de 3/8” x 3 ¾ ”. 200Kg/cm2 de resistencia.</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>COL-AB-10-00 0 22/07/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>Medidas Capacidad Área Mínima Edad (años)</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>COLUMPIO RESIDENCIAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>COLUMPIOS 2.60m x 1.60m x 2.00m 2niños 6.20m x 5.20m 4-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>Descripción de producto</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>Columpio Residencial de 2 asientos de banda en plástico y</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>cadena galvanizada de ¼” . Esta fabricado en tubo redondo</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>NGR Ced.30 Norma ASTM-A-513. Ideal para cualquier</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>espacio.</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>Sujeción y Unión</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>Utilización de soldadura MIGG (GMAW), para la unión de</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>los elementos de un componente en acero. Sujeción</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>accesorios mediante tornillos tipo "Torks", tuercas inserto</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>nylon, tuercas de presión y aplicación de "LocTite”, lo cual</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>dificulta la extracción y el vandalismo.</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>Recubrimiento</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>Las partes en acero pasan por un tratamiento de superficie</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>de tres etapas para evitar la oxidación natural del acero:</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>Fosfatodesengrase, enjuague y sellado, el cual evita la</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>oxidación natural del acero. Se les aplica un recubrimiento</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>de pintura poliéster electrostático en polvo (PowderCoating)</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>con una temperatura de curado a 200° C. lo cual asegura la</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>adherencia, la dureza y el brillo del recubrimiento sobre el</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>Imagen de referencia, puede haber variación</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>producto.</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>2.00m</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>1.60m 2.60m</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>Dimensiones de referencia, puede haber variaciones.</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>VARIANTES DE ANCLAJE</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>ANCLADO EN CEMENTO:</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>TAQUETEADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>• Realizar hoyos de 40cm de</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>• El concreto a usar debe ser de 200 Kg/cm2 Diámetro.</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>de resistencia. • Excavar a 30cm de profundidad para</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>• El espesor mínimo de la plancha de enterrar postes y accesorios.</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>concreto debe ser de 15cm. • Rellenar hoyos con un concreto de</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>• Usar taquetes expansivos de 3/8” x 3 ¾ ”. 200Kg/cm2 de resistencia.</t>
         </is>
       </c>
     </row>

</xml_diff>